<commit_message>
updated analyses for 13th
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-13.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-13.xlsx
@@ -1337,15 +1337,9 @@
     <t>Routing at DUS Signal 2N</t>
   </si>
   <si>
-    <t>Routing at DUS (southbound signals)</t>
-  </si>
-  <si>
     <t>Premature downgrade at EC0629XH 63-1T 1S</t>
   </si>
   <si>
-    <t>Tentative</t>
-  </si>
-  <si>
     <t>Investigating</t>
   </si>
   <si>
@@ -1403,22 +1397,28 @@
     <t>Wi-MAX outage</t>
   </si>
   <si>
-    <t>Premature downgrade at EC0508RH 43-1T 1N</t>
-  </si>
-  <si>
     <t>No issue found in logs, no issue found in service log. Signals ahead were all PROCEED CAB. GPS was acceptable. Not sure why a cut out happened here.</t>
   </si>
   <si>
-    <t>Routing @ Pena, MAP DISAPPEARED</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>Link failures to 78th</t>
   </si>
   <si>
     <t>Link failures to 61st</t>
+  </si>
+  <si>
+    <t>DUS WIU was not beaconing statuses. Maintenance?</t>
+  </si>
+  <si>
+    <t>Routing at DUS 2S</t>
+  </si>
+  <si>
+    <t>Comparator issue caused train comm outage</t>
+  </si>
+  <si>
+    <t>Train was cut out by message from TMDS at 05-13-2016 17:31:42.799</t>
+  </si>
+  <si>
+    <t>Onboard in-route failure</t>
   </si>
 </sst>
 </file>
@@ -1909,7 +1909,238 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2313,8 +2544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK171"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R131" sqref="R131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,10 +2871,10 @@
         <v>34</v>
       </c>
       <c r="Q4" s="62" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="R4" s="62" t="s">
-        <v>426</v>
+        <v>450</v>
       </c>
       <c r="T4" s="74" t="str">
         <f t="shared" ref="T4:T35" si="10">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E4-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I4+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B4&amp;"%22')),sort:!(Time,asc))"</f>
@@ -2811,10 +3042,10 @@
         <v>35</v>
       </c>
       <c r="Q6" s="62" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="R6" s="62" t="s">
-        <v>426</v>
+        <v>450</v>
       </c>
       <c r="T6" s="74" t="str">
         <f t="shared" si="10"/>
@@ -5332,7 +5563,7 @@
         <v>3.3333333267364651</v>
       </c>
       <c r="Q36" s="62" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="R36" s="62" t="s">
         <v>426</v>
@@ -8275,10 +8506,10 @@
         <v>39.916666662320495</v>
       </c>
       <c r="Q71" s="62" t="s">
-        <v>429</v>
+        <v>142</v>
       </c>
       <c r="R71" s="62" t="s">
-        <v>427</v>
+        <v>447</v>
       </c>
       <c r="T71" s="74" t="str">
         <f t="shared" si="28"/>
@@ -9455,10 +9686,10 @@
         <v>43.016666664043441</v>
       </c>
       <c r="Q85" s="62" t="s">
-        <v>429</v>
+        <v>142</v>
       </c>
       <c r="R85" s="62" t="s">
-        <v>427</v>
+        <v>451</v>
       </c>
       <c r="T85" s="74" t="str">
         <f t="shared" si="28"/>
@@ -9962,10 +10193,10 @@
         <v>48</v>
       </c>
       <c r="Q91" s="62" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="R91" s="62" t="s">
-        <v>428</v>
+        <v>452</v>
       </c>
       <c r="T91" s="74" t="str">
         <f t="shared" si="28"/>
@@ -10131,10 +10362,10 @@
         <v>45.83333333954215</v>
       </c>
       <c r="Q93" s="62" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="R93" s="62" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="T93" s="74" t="str">
         <f t="shared" si="28"/>
@@ -10807,7 +11038,7 @@
         <v>142</v>
       </c>
       <c r="R101" s="62" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="T101" s="74" t="str">
         <f t="shared" si="38"/>
@@ -11312,10 +11543,10 @@
         <v>39.366666680434719</v>
       </c>
       <c r="Q107" s="62" t="s">
-        <v>452</v>
+        <v>142</v>
       </c>
       <c r="R107" s="62" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="T107" s="74" t="str">
         <f t="shared" si="38"/>
@@ -12069,10 +12300,10 @@
         <v>38.283333334838971</v>
       </c>
       <c r="Q116" s="62" t="s">
-        <v>429</v>
+        <v>142</v>
       </c>
       <c r="R116" s="62" t="s">
-        <v>427</v>
+        <v>447</v>
       </c>
       <c r="T116" s="74" t="str">
         <f t="shared" si="38"/>
@@ -12244,7 +12475,7 @@
         <v>142</v>
       </c>
       <c r="R118" s="62" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="T118" s="74" t="str">
         <f t="shared" si="38"/>
@@ -12998,10 +13229,10 @@
         <v>44.283333333441988</v>
       </c>
       <c r="Q127" s="62" t="s">
-        <v>429</v>
+        <v>142</v>
       </c>
       <c r="R127" s="62" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="T127" s="74" t="str">
         <f t="shared" si="38"/>
@@ -13170,7 +13401,7 @@
         <v>142</v>
       </c>
       <c r="R129" s="62" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="T129" s="74" t="str">
         <f t="shared" si="38"/>
@@ -13255,10 +13486,10 @@
         <v>87.883333330973983</v>
       </c>
       <c r="Q130" s="62" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="R130" s="62" t="s">
-        <v>432</v>
+        <v>454</v>
       </c>
       <c r="T130" s="74" t="str">
         <f t="shared" si="38"/>
@@ -13505,10 +13736,10 @@
         <v>37.566666668280959</v>
       </c>
       <c r="Q133" s="62" t="s">
-        <v>429</v>
+        <v>142</v>
       </c>
       <c r="R133" s="62" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="T133" s="74" t="str">
         <f t="shared" si="48"/>
@@ -14687,7 +14918,7 @@
         <v>142</v>
       </c>
       <c r="R147" s="62" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T147" s="74" t="str">
         <f t="shared" si="48"/>
@@ -15794,28 +16025,28 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 U2 U3:V1048576">
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1 V3:V1048576">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155:P155 A3:R154">
-    <cfRule type="expression" dxfId="13" priority="34">
+    <cfRule type="expression" dxfId="46" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="35">
+    <cfRule type="expression" dxfId="45" priority="35">
       <formula>$O3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q155:R155">
-    <cfRule type="expression" dxfId="11" priority="76">
+    <cfRule type="expression" dxfId="44" priority="76">
       <formula>$P155&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="77">
+    <cfRule type="expression" dxfId="43" priority="77">
       <formula>$O174&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15974,7 +16205,7 @@
         <v>96</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16019,7 +16250,7 @@
         <v>96</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16064,7 +16295,7 @@
         <v>166</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16109,7 +16340,7 @@
         <v>96</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16154,7 +16385,7 @@
         <v>96</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16199,7 +16430,7 @@
         <v>166</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16244,7 +16475,7 @@
         <v>166</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16289,7 +16520,7 @@
         <v>166</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16334,7 +16565,7 @@
         <v>166</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16379,7 +16610,7 @@
         <v>166</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -18873,17 +19104,17 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N2 M2:M1048576">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11:N12 B69:N70 B66:K68 N66:N68 L29:M68 M8:M12 M8:N10 M13:N28 B8:L28 B3:N7">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="40" priority="6">
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:K65 N29:N65">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="39" priority="3">
       <formula>$M29="Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19014,7 +19245,7 @@
         <v>1360000</v>
       </c>
       <c r="E3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -19065,7 +19296,7 @@
         <v>1430000</v>
       </c>
       <c r="E6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -19235,7 +19466,7 @@
         <v>1120000</v>
       </c>
       <c r="E16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -19252,7 +19483,7 @@
         <v>1460000</v>
       </c>
       <c r="E17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -19286,7 +19517,7 @@
         <v>1120000</v>
       </c>
       <c r="E19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -19371,7 +19602,7 @@
         <v>1360000</v>
       </c>
       <c r="E24" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -19405,7 +19636,7 @@
         <v>1110000</v>
       </c>
       <c r="E26" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -19422,7 +19653,7 @@
         <v>1110000</v>
       </c>
       <c r="E27" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -19507,7 +19738,7 @@
         <v>1430000</v>
       </c>
       <c r="E32" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -19677,7 +19908,7 @@
         <v>1520000</v>
       </c>
       <c r="E42" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -19685,7 +19916,7 @@
         <v>42503.20952546296</v>
       </c>
       <c r="B43" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C43" t="s">
         <v>202</v>
@@ -19694,7 +19925,7 @@
         <v>1430000</v>
       </c>
       <c r="E43" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -19702,7 +19933,7 @@
         <v>42503.727569444447</v>
       </c>
       <c r="B44" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C44" t="s">
         <v>355</v>
@@ -19745,7 +19976,7 @@
         <v>950000</v>
       </c>
       <c r="E46" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -19762,7 +19993,7 @@
         <v>1360000</v>
       </c>
       <c r="E47" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -19813,7 +20044,7 @@
         <v>950000</v>
       </c>
       <c r="E50" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -19855,7 +20086,7 @@
         <v>42503.285497685189</v>
       </c>
       <c r="B53" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C53" t="s">
         <v>220</v>
@@ -19864,7 +20095,7 @@
         <v>1430000</v>
       </c>
       <c r="E53" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -19881,7 +20112,7 @@
         <v>950000</v>
       </c>
       <c r="E54" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -19923,7 +20154,7 @@
         <v>42503.506724537037</v>
       </c>
       <c r="B57" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C57" t="s">
         <v>279</v>
@@ -19949,7 +20180,7 @@
         <v>1520000</v>
       </c>
       <c r="E58" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -20034,7 +20265,7 @@
         <v>1110000</v>
       </c>
       <c r="E63" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -20221,7 +20452,7 @@
         <v>950000</v>
       </c>
       <c r="E74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -20289,7 +20520,7 @@
         <v>1110000</v>
       </c>
       <c r="E78" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -20340,7 +20571,7 @@
         <v>1430000</v>
       </c>
       <c r="E81" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -20357,7 +20588,7 @@
         <v>1110000</v>
       </c>
       <c r="E82" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -20391,7 +20622,7 @@
         <v>1460000</v>
       </c>
       <c r="E84" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -20408,7 +20639,7 @@
         <v>1430000</v>
       </c>
       <c r="E85" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -20416,7 +20647,7 @@
         <v>42503.433530092596</v>
       </c>
       <c r="B86" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C86" t="s">
         <v>260</v>
@@ -20442,7 +20673,7 @@
         <v>1110000</v>
       </c>
       <c r="E87" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -20476,7 +20707,7 @@
         <v>1360000</v>
       </c>
       <c r="E89" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -20493,7 +20724,7 @@
         <v>950000</v>
       </c>
       <c r="E90" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -20527,7 +20758,7 @@
         <v>1110000</v>
       </c>
       <c r="E92" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -20544,7 +20775,7 @@
         <v>1430000</v>
       </c>
       <c r="E93" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -20578,7 +20809,7 @@
         <v>1110000</v>
       </c>
       <c r="E95" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -20612,7 +20843,7 @@
         <v>1360000</v>
       </c>
       <c r="E97" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -20663,7 +20894,7 @@
         <v>1430000</v>
       </c>
       <c r="E100" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -20697,7 +20928,7 @@
         <v>1120000</v>
       </c>
       <c r="E102" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -20714,7 +20945,7 @@
         <v>1360000</v>
       </c>
       <c r="E103" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -20765,7 +20996,7 @@
         <v>1430000</v>
       </c>
       <c r="E106" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -20833,7 +21064,7 @@
         <v>1520000</v>
       </c>
       <c r="E110" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -20850,7 +21081,7 @@
         <v>950000</v>
       </c>
       <c r="E111" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -20901,7 +21132,7 @@
         <v>1520000</v>
       </c>
       <c r="E114" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -20918,7 +21149,7 @@
         <v>1120000</v>
       </c>
       <c r="E115" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -20952,7 +21183,7 @@
         <v>950000</v>
       </c>
       <c r="E117" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -20986,7 +21217,7 @@
         <v>900000</v>
       </c>
       <c r="E119" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -21173,7 +21404,7 @@
         <v>1120000</v>
       </c>
       <c r="E130" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -21207,7 +21438,7 @@
         <v>950000</v>
       </c>
       <c r="E132" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -21235,13 +21466,13 @@
         <v>127</v>
       </c>
       <c r="C134" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D134">
         <v>900000</v>
       </c>
       <c r="E134" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -21258,7 +21489,7 @@
         <v>1120000</v>
       </c>
       <c r="E135" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -21292,7 +21523,7 @@
         <v>900000</v>
       </c>
       <c r="E137" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -21334,7 +21565,7 @@
         <v>42503.57984953704</v>
       </c>
       <c r="B140" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C140" t="s">
         <v>301</v>
@@ -21360,7 +21591,7 @@
         <v>1520000</v>
       </c>
       <c r="E141" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -21411,7 +21642,7 @@
         <v>1360000</v>
       </c>
       <c r="E144" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -21428,7 +21659,7 @@
         <v>1120000</v>
       </c>
       <c r="E145" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -21436,7 +21667,7 @@
         <v>42503.358703703707</v>
       </c>
       <c r="B146" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C146" t="s">
         <v>240</v>
@@ -21445,7 +21676,7 @@
         <v>1430000</v>
       </c>
       <c r="E146" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -21521,7 +21752,7 @@
         <v>42503.65388888889</v>
       </c>
       <c r="B151" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C151" t="s">
         <v>330</v>
@@ -21581,7 +21812,7 @@
         <v>1120000</v>
       </c>
       <c r="E154" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -21751,7 +21982,7 @@
         <v>1360000</v>
       </c>
       <c r="E164" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update some routing stuff
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-13.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-13.xlsx
@@ -1397,13 +1397,13 @@
     <t>Onboard in-route failure</t>
   </si>
   <si>
-    <t>DUS hardware issues</t>
-  </si>
-  <si>
     <t>Train went backwards for unknown reasons. Operator error?</t>
   </si>
   <si>
     <t>Discuss</t>
+  </si>
+  <si>
+    <t>DUS routing issue</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1894,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2256,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK171"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R107" sqref="R107"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R85" sqref="R85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2586,7 +2649,7 @@
         <v>142</v>
       </c>
       <c r="R4" s="62" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="T4" s="74" t="str">
         <f t="shared" ref="T4:T35" si="10">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E4-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I4+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B4&amp;"%22')),sort:!(Time,asc))"</f>
@@ -2757,7 +2820,7 @@
         <v>142</v>
       </c>
       <c r="R6" s="62" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="T6" s="74" t="str">
         <f t="shared" si="10"/>
@@ -5278,7 +5341,7 @@
         <v>142</v>
       </c>
       <c r="R36" s="62" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="T36" s="74" t="str">
         <f t="shared" ref="T36:T67" si="19">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E36-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I36+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B36&amp;"%22')),sort:!(Time,asc))"</f>
@@ -9401,7 +9464,7 @@
         <v>142</v>
       </c>
       <c r="R85" s="62" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="T85" s="74" t="str">
         <f t="shared" si="28"/>
@@ -13198,10 +13261,10 @@
         <v>87.883333330973983</v>
       </c>
       <c r="Q130" s="62" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="R130" s="62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="T130" s="74" t="str">
         <f t="shared" si="38"/>
@@ -15737,28 +15800,28 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 U2 U3:V1048576">
-    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1 V3:V1048576">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155:P155 A3:R154">
-    <cfRule type="expression" dxfId="7" priority="34">
+    <cfRule type="expression" dxfId="16" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="35">
+    <cfRule type="expression" dxfId="15" priority="35">
       <formula>$O3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q155:R155">
-    <cfRule type="expression" dxfId="5" priority="76">
+    <cfRule type="expression" dxfId="14" priority="76">
       <formula>$P155&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="77">
+    <cfRule type="expression" dxfId="13" priority="77">
       <formula>$O174&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18816,17 +18879,17 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N2 M2:M1048576">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11:N12 B69:N70 B66:K68 N66:N68 L29:M68 M8:M12 M8:N10 M13:N28 B8:L28 B3:N7">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:K65 N29:N65">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>$M29="Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update notes on DUS events
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-13.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-13.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="452">
   <si>
     <t>Train ID</t>
   </si>
@@ -1403,7 +1403,13 @@
     <t>Discuss</t>
   </si>
   <si>
-    <t>DUS routing issue</t>
+    <t>DUS was not communicating with back office</t>
+  </si>
+  <si>
+    <t>DUS routing issue (2N signal was STOP during entire event)</t>
+  </si>
+  <si>
+    <t>DUS routing issue (4S signal was STOP during entire event)</t>
   </si>
 </sst>
 </file>
@@ -1894,70 +1900,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -2319,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK171"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R85" sqref="R85"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5341,7 +5284,7 @@
         <v>142</v>
       </c>
       <c r="R36" s="62" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="T36" s="74" t="str">
         <f t="shared" ref="T36:T67" si="19">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E36-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I36+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B36&amp;"%22')),sort:!(Time,asc))"</f>
@@ -9464,7 +9407,7 @@
         <v>142</v>
       </c>
       <c r="R85" s="62" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="T85" s="74" t="str">
         <f t="shared" si="28"/>
@@ -15800,28 +15743,28 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 U2 U3:V1048576">
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1 V3:V1048576">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A155:P155 A3:R154">
-    <cfRule type="expression" dxfId="16" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="35">
+    <cfRule type="expression" dxfId="6" priority="35">
       <formula>$O3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q155:R155">
-    <cfRule type="expression" dxfId="14" priority="76">
+    <cfRule type="expression" dxfId="5" priority="76">
       <formula>$P155&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="77">
+    <cfRule type="expression" dxfId="4" priority="77">
       <formula>$O174&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18879,17 +18822,17 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N2 M2:M1048576">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11:N12 B69:N70 B66:K68 N66:N68 L29:M68 M8:M12 M8:N10 M13:N28 B8:L28 B3:N7">
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:K65 N29:N65">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$M29="Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>